<commit_message>
editado planilha com filiais
</commit_message>
<xml_diff>
--- a/Data/Filiais.xlsx
+++ b/Data/Filiais.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Robos\prj_SVR_Confirmar_Agenda\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5AEC8F3-D33D-450F-BCA6-F0A2D5ECC20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D460E36C-3868-4FB0-8C18-B131637FA493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9CEABD6A-CE4A-4AC6-9E90-C7BB17EA36C2}"/>
   </bookViews>
   <sheets>
-    <sheet name="base" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="73">
   <si>
     <t>AGR</t>
   </si>
@@ -607,11 +607,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CECDE297-80A8-4DC2-9817-2F1F146F9C67}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -632,6 +630,30 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
planilha com as filiais que o robo irá rodar
</commit_message>
<xml_diff>
--- a/Data/Filiais.xlsx
+++ b/Data/Filiais.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Robos\prj_SVR_Confirmar_Agenda\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BDC3B15-B8B6-4F8F-80E9-574F56DB5923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9269AE8B-4FA5-4028-88CB-AA89A5F6BB6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9CEABD6A-CE4A-4AC6-9E90-C7BB17EA36C2}"/>
+    <workbookView xWindow="29760" yWindow="2910" windowWidth="15375" windowHeight="7815" xr2:uid="{9CEABD6A-CE4A-4AC6-9E90-C7BB17EA36C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="73">
   <si>
     <t>AGR</t>
   </si>
@@ -607,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CECDE297-80A8-4DC2-9817-2F1F146F9C67}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A3" sqref="A3:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -629,34 +629,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>